<commit_message>
bug fix with edit user ad
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -673,7 +673,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -771,7 +771,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>56</v>
@@ -1268,7 +1268,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>

<commit_message>
edit user profile done
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -683,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,7 +771,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="6">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>56</v>
@@ -1007,7 +1007,7 @@
         <v>22</v>
       </c>
       <c r="C29" s="5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>5</v>
@@ -1268,7 +1268,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>